<commit_message>
Updated Report and Test Files
</commit_message>
<xml_diff>
--- a/Results/Parallel - CUDA.xlsx
+++ b/Results/Parallel - CUDA.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suttie\Desktop\Projects\C++ Projects\N-Queens-CW2\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CCEEB3-7E08-497E-A25A-AEDD18003563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CBC61-4D7B-4502-BB6E-0F99F15CAD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>RUN 1</t>
   </si>
@@ -79,6 +88,12 @@
   </si>
   <si>
     <t>N = 10</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CUDA</t>
   </si>
 </sst>
 </file>
@@ -134,6 +149,1054 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>N-Queens CUDA Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CUDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$14:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>N = 4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>N = 5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>N = 6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>N = 7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>N = 8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>N = 9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>N = 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.3419999999999991E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9218000000000005E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9339999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4494999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7079000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12924319999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.613448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D023-41B1-9343-BEA94A8CF8B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1738773744"/>
+        <c:axId val="1738772496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1738773744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> COMPLEXITY</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1738772496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1738772496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>TIME</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (SECONDS)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1738773744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028B8EE9-F4BF-445A-B09B-451CA4547A3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,13 +1462,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
@@ -447,38 +1513,376 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="1">
+        <v>5.8600000000000004E-4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7.0299999999999996E-4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7.5600000000000005E-4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5.3799999999999996E-4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6.2200000000000005E-4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.11E-4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6.5099999999999999E-4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6.7599999999999995E-4</v>
+      </c>
+      <c r="J2" s="1">
+        <v>6.7199999999999996E-4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>5.2700000000000002E-4</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(B2:K2)</f>
+        <v>6.3419999999999991E-4</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="1">
+        <v>5.2300000000000003E-4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.4579999999999999E-4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5.9100000000000005E-4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4.55E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.8299999999999998E-4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.22E-4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4.28E-4</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5.5099999999999995E-4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4.7800000000000002E-4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4.4499999999999997E-4</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(B3:K3)</f>
+        <v>4.9218000000000005E-4</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="1">
+        <v>5.4699999999999996E-4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.2499999999999998E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.86E-4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4.2700000000000002E-4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.3600000000000003E-4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6.1799999999999995E-4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4.8299999999999998E-4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5.04E-4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4.8899999999999996E-4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.1900000000000004E-4</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE(B4:K4)</f>
+        <v>4.9339999999999996E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="1">
+        <v>7.0800000000000004E-3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.0600000000000003E-4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.5500000000000003E-4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7.1299999999999998E-4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.9499999999999998E-4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.139E-3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>8.1999999999999998E-4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.6600000000000002E-4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>7.76E-4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9.4499999999999998E-4</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE(B5:K5)</f>
+        <v>1.4494999999999998E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" s="1">
+        <v>3.5379999999999999E-3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.588E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.715E-3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.6480000000000002E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.5729999999999998E-3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.8930000000000002E-3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3.5349999999999999E-3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.1070000000000004E-3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3.6809999999999998E-3</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3.8010000000000001E-3</v>
+      </c>
+      <c r="L6">
+        <f>AVERAGE(B6:K6)</f>
+        <v>3.7079000000000001E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="1">
+        <v>6.7359000000000002E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.67908999999999997</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.8704000000000001E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.7985000000000004E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6.8915000000000004E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.8678000000000003E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6.7320000000000005E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6.8461999999999995E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>6.7766000000000007E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>6.8153000000000005E-2</v>
+      </c>
+      <c r="L7">
+        <f>AVERAGE(B7:K7)</f>
+        <v>0.12924319999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="1">
+        <v>1.6193</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.62233</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.6218999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.6124099999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.65421</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.6092</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.59921</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1.5967499999999999</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.5910899999999999</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.60808</v>
+      </c>
+      <c r="L8">
+        <f>AVERAGE(B8:K8)</f>
+        <v>1.613448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B2:K2)</f>
+        <v>6.3419999999999991E-4</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B3:K3)</f>
+        <v>4.9218000000000005E-4</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <f>AVERAGE(B4:K4)</f>
+        <v>4.9339999999999996E-4</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(B5:K5)</f>
+        <v>1.4494999999999998E-3</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <f>AVERAGE(B6:K6)</f>
+        <v>3.7079000000000001E-3</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <f>AVERAGE(B7:K7)</f>
+        <v>0.12924319999999997</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(B8:K8)</f>
+        <v>1.613448</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>